<commit_message>
Actualizacion de Excel, Nuev medida y enfoque
</commit_message>
<xml_diff>
--- a/back-end/Web Presentacion/Web Dinamico/MRVMinem/bin/Documentos/1.7 Plantilla_Lamparas_de_alumbrado_publico.xlsx
+++ b/back-end/Web Presentacion/Web Dinamico/MRVMinem/bin/Documentos/1.7 Plantilla_Lamparas_de_alumbrado_publico.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JK\Downloads\PLANTILLA_MINEN\CONECTADO\ORDENADO\git-new-repository\back-end\Web Dinamico\MRVMinem\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E071B9B-8709-41E5-A45A-A3E97705958C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{048E799F-1FF6-4BDA-9D71-D92380C958E8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20295" windowHeight="1995"/>
   </bookViews>
   <sheets>
     <sheet name="Lampara de Alumbrado Electrico" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="Lista_Mes">Hoja2!$C$3:$C$14</definedName>
     <definedName name="Tabla_Mes">Hoja2!$C$3:$D$14</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Dell</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AE85AC85-F1B2-4D29-9302-D73FDD35681A}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C48B2F1A-3C74-4462-896D-4685EA0A4A18}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{4E688767-F91D-4884-A025-997ADD0B63B5}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{240E81DE-B2DE-4367-B9D5-DC5EDA77C9DB}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{4CD05B8C-AFB5-482F-9460-3923FFC54572}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{6A498BF0-D5D0-423F-8040-61CAFB2A0B74}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -136,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Año</t>
   </si>
@@ -201,7 +200,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
@@ -622,8 +621,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7422B1-01C7-47CE-A90F-DE7B5133F9DA}">
-  <dimension ref="A1:G311"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -678,7 +677,7 @@
         <v>150000</v>
       </c>
       <c r="F2" s="5">
-        <f t="shared" ref="F2:F65" si="0">VLOOKUP(G2,Tabla_Mes,2,)</f>
+        <f t="shared" ref="F2:F63" si="0">VLOOKUP(G2,Tabla_Mes,2,)</f>
         <v>4</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -686,40 +685,28 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2013</v>
-      </c>
-      <c r="B3" s="6">
-        <v>41333</v>
-      </c>
-      <c r="C3" s="5">
-        <v>250</v>
-      </c>
-      <c r="D3" s="5">
-        <v>120</v>
-      </c>
-      <c r="E3" s="5">
-        <v>110000</v>
-      </c>
-      <c r="F3" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G4" s="5"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
@@ -1436,7 +1423,7 @@
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F64:F127" si="1">VLOOKUP(G64,Tabla_Mes,2,)</f>
         <v>#N/A</v>
       </c>
       <c r="G64" s="3"/>
@@ -1448,7 +1435,7 @@
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="G65" s="3"/>
@@ -1460,7 +1447,7 @@
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3" t="e">
-        <f t="shared" ref="F66:F129" si="1">VLOOKUP(G66,Tabla_Mes,2,)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="G66" s="3"/>
@@ -2204,7 +2191,7 @@
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F128:F191" si="2">VLOOKUP(G128,Tabla_Mes,2,)</f>
         <v>#N/A</v>
       </c>
       <c r="G128" s="3"/>
@@ -2216,7 +2203,7 @@
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="G129" s="3"/>
@@ -2228,7 +2215,7 @@
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
       <c r="F130" s="3" t="e">
-        <f t="shared" ref="F130:F193" si="2">VLOOKUP(G130,Tabla_Mes,2,)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="G130" s="3"/>
@@ -2972,7 +2959,7 @@
       <c r="D192" s="3"/>
       <c r="E192" s="3"/>
       <c r="F192" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F192:F255" si="3">VLOOKUP(G192,Tabla_Mes,2,)</f>
         <v>#N/A</v>
       </c>
       <c r="G192" s="3"/>
@@ -2984,7 +2971,7 @@
       <c r="D193" s="3"/>
       <c r="E193" s="3"/>
       <c r="F193" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="G193" s="3"/>
@@ -2996,7 +2983,7 @@
       <c r="D194" s="3"/>
       <c r="E194" s="3"/>
       <c r="F194" s="3" t="e">
-        <f t="shared" ref="F194:F257" si="3">VLOOKUP(G194,Tabla_Mes,2,)</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="G194" s="3"/>
@@ -3740,7 +3727,7 @@
       <c r="D256" s="3"/>
       <c r="E256" s="3"/>
       <c r="F256" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F256:F308" si="4">VLOOKUP(G256,Tabla_Mes,2,)</f>
         <v>#N/A</v>
       </c>
       <c r="G256" s="3"/>
@@ -3752,7 +3739,7 @@
       <c r="D257" s="3"/>
       <c r="E257" s="3"/>
       <c r="F257" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="G257" s="3"/>
@@ -3764,7 +3751,7 @@
       <c r="D258" s="3"/>
       <c r="E258" s="3"/>
       <c r="F258" s="3" t="e">
-        <f t="shared" ref="F258:F310" si="4">VLOOKUP(G258,Tabla_Mes,2,)</f>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="G258" s="3"/>
@@ -4371,45 +4358,21 @@
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309" s="3"/>
-      <c r="B309" s="4"/>
+      <c r="B309" s="3"/>
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
       <c r="E309" s="3"/>
-      <c r="F309" s="3" t="e">
-        <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
+      <c r="F309" s="3"/>
       <c r="G309" s="3"/>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A310" s="3"/>
-      <c r="B310" s="4"/>
-      <c r="C310" s="3"/>
-      <c r="D310" s="3"/>
-      <c r="E310" s="3"/>
-      <c r="F310" s="3" t="e">
-        <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G310" s="3"/>
-    </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A311" s="3"/>
-      <c r="B311" s="3"/>
-      <c r="C311" s="3"/>
-      <c r="D311" s="3"/>
-      <c r="E311" s="3"/>
-      <c r="F311" s="3"/>
-      <c r="G311" s="3"/>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ZnyR2Piho5vrfl2ER66aGoVSPVinZPn1W+VqxH6fDX1FIttc2Apmfn92CU/mN/S5rI60kfOmIPBUvK3EWY8vYA==" saltValue="COSDsspbJdCM73h18KnZcA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="BZE4tIVOLPiP0rKaXoetfVj/d+HaC6mld2O26iC/1ZYkm+pxn1dGGrYO991RPF7xtkmtSY7BCxXiB1uS2qjwyQ==" saltValue="Xs5RY7x2g5KlXn6rrzpXow==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A310" xr:uid="{EFABA8EB-ADB9-49A2-84A8-8D15D3266206}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A308">
       <formula1>Lista_Anno</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G310" xr:uid="{AEDA1AB1-8B4D-4618-858A-ED22066845BD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G308">
       <formula1>Lista_Mes</formula1>
     </dataValidation>
   </dataValidations>
@@ -4420,7 +4383,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C831AF49-9B93-4231-A6A7-BA1194CC59F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>